<commit_message>
add new Component and Components properties
</commit_message>
<xml_diff>
--- a/sanitation/utils/default_components.xlsx
+++ b/sanitation/utils/default_components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation/sanitation/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{E1336E32-95D7-434C-A5D7-E83C4F520CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B658585-71C4-154E-ACEF-9119612C6A16}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{E1336E32-95D7-434C-A5D7-E83C4F520CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DBB82F0-402A-6743-8A48-E7C3E1D18654}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="3120" windowWidth="27640" windowHeight="16940" xr2:uid="{0F5A49EB-0145-7C4A-9641-FECB1B40263B}"/>
+    <workbookView xWindow="7440" yWindow="4660" windowWidth="27640" windowHeight="16940" xr2:uid="{0F5A49EB-0145-7C4A-9641-FECB1B40263B}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -523,6 +523,33 @@
   </si>
   <si>
     <t>i_charge</t>
+  </si>
+  <si>
+    <t>i_C</t>
+  </si>
+  <si>
+    <t>i_N</t>
+  </si>
+  <si>
+    <t>i_P</t>
+  </si>
+  <si>
+    <t>i_K</t>
+  </si>
+  <si>
+    <t>i_mass</t>
+  </si>
+  <si>
+    <t>f_BOD5_COD</t>
+  </si>
+  <si>
+    <t>f_uBOD_COD</t>
+  </si>
+  <si>
+    <t>f_Vmass_Totmass</t>
+  </si>
+  <si>
+    <t>measure_unit</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAC1A27-BC0D-234D-8D38-3B5D0C6F117B}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,13 +1038,13 @@
     <col min="1" max="1" width="11.5" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="17.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="4" max="12" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="58.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="17.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,22 +1055,49 @@
         <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1056,20 +1110,45 @@
       <c r="D2" s="4">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="O2" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1082,20 +1161,45 @@
       <c r="D3" s="13">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="13" t="b">
+      <c r="P3" s="13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q3" s="13"/>
+    </row>
+    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>142</v>
       </c>
@@ -1108,20 +1212,45 @@
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="O4" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>145</v>
       </c>
@@ -1134,20 +1263,45 @@
       <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H5" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
@@ -1160,20 +1314,45 @@
       <c r="D6" s="17">
         <v>0</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>0</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="17">
+        <v>0</v>
+      </c>
+      <c r="M6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="N6" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="O6" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="19" t="b">
+      <c r="P6" s="19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
@@ -1184,22 +1363,47 @@
         <v>161</v>
       </c>
       <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
         <v>-1</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="N7" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="O7" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H7" s="16" t="b">
+      <c r="P7" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q7" s="16"/>
+    </row>
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -1212,20 +1416,45 @@
       <c r="D8" s="13">
         <v>0</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="N8" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="O8" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H8" s="16" t="b">
+      <c r="P8" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -1236,22 +1465,47 @@
         <v>161</v>
       </c>
       <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
         <v>-1</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="N9" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="O9" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="16" t="b">
+      <c r="P9" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
@@ -1264,20 +1518,45 @@
       <c r="D10" s="13">
         <v>0</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="13">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0</v>
+      </c>
+      <c r="L10" s="13">
+        <v>0</v>
+      </c>
+      <c r="M10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="N10" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="O10" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H10" s="16" t="b">
+      <c r="P10" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -1288,20 +1567,45 @@
       <c r="D11" s="13">
         <v>0</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="O11" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H11" s="16" t="b">
+      <c r="P11" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q11" s="16"/>
+    </row>
+    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
@@ -1312,20 +1616,45 @@
       <c r="D12" s="13">
         <v>0</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0</v>
+      </c>
+      <c r="M12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="N12" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="O12" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="16" t="b">
+      <c r="P12" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
@@ -1336,20 +1665,45 @@
       <c r="D13" s="7">
         <v>0</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="O13" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H13" s="9" t="b">
+      <c r="P13" s="9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>97</v>
       </c>
@@ -1360,22 +1714,47 @@
         <v>161</v>
       </c>
       <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
         <v>1</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="N14" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="O14" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="H14" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="19"/>
+    </row>
+    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>100</v>
       </c>
@@ -1388,20 +1767,45 @@
       <c r="D15" s="13">
         <v>0</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="M15" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="N15" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="O15" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H15" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="16"/>
+    </row>
+    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>103</v>
       </c>
@@ -1412,22 +1816,47 @@
         <v>161</v>
       </c>
       <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
         <v>-2</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0</v>
+      </c>
+      <c r="M16" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="N16" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="O16" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H16" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="16"/>
+    </row>
+    <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>106</v>
       </c>
@@ -1440,20 +1869,45 @@
       <c r="D17" s="13">
         <v>0</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="13">
+        <v>0</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13">
+        <v>0</v>
+      </c>
+      <c r="M17" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="N17" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="O17" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H17" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="16"/>
+    </row>
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>109</v>
       </c>
@@ -1464,22 +1918,47 @@
         <v>161</v>
       </c>
       <c r="D18" s="13">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
         <v>-1</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
+        <v>0</v>
+      </c>
+      <c r="M18" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="N18" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="O18" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H18" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="16"/>
+    </row>
+    <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>112</v>
       </c>
@@ -1492,20 +1971,45 @@
       <c r="D19" s="13">
         <v>0</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="13">
+        <v>0</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
+        <v>0</v>
+      </c>
+      <c r="M19" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="N19" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="O19" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H19" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="16"/>
+    </row>
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>115</v>
       </c>
@@ -1516,22 +2020,47 @@
         <v>161</v>
       </c>
       <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
         <v>-1</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
+        <v>0</v>
+      </c>
+      <c r="M20" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="N20" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="O20" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H20" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P20" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="16"/>
+    </row>
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>118</v>
       </c>
@@ -1542,22 +2071,47 @@
         <v>161</v>
       </c>
       <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
         <v>-2</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
+        <v>0</v>
+      </c>
+      <c r="M21" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="N21" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="O21" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H21" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>121</v>
       </c>
@@ -1568,22 +2122,47 @@
         <v>161</v>
       </c>
       <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
         <v>-3</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="N22" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="O22" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H22" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P22" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="16"/>
+    </row>
+    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>124</v>
       </c>
@@ -1594,22 +2173,47 @@
         <v>161</v>
       </c>
       <c r="D23" s="20">
+        <v>0</v>
+      </c>
+      <c r="E23" s="20">
+        <v>0</v>
+      </c>
+      <c r="F23" s="20">
+        <v>0</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
         <v>1</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="J23" s="20">
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0</v>
+      </c>
+      <c r="L23" s="20">
+        <v>0</v>
+      </c>
+      <c r="M23" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="N23" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="O23" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H23" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P23" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="16"/>
+    </row>
+    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>127</v>
       </c>
@@ -1620,22 +2224,47 @@
         <v>161</v>
       </c>
       <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="20">
+        <v>0</v>
+      </c>
+      <c r="F24" s="20">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0</v>
+      </c>
+      <c r="H24" s="20">
+        <v>0</v>
+      </c>
+      <c r="I24" s="20">
         <v>2</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="J24" s="20">
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
+        <v>0</v>
+      </c>
+      <c r="M24" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="N24" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="O24" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H24" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P24" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="16"/>
+    </row>
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>130</v>
       </c>
@@ -1646,22 +2275,47 @@
         <v>161</v>
       </c>
       <c r="D25" s="20">
+        <v>0</v>
+      </c>
+      <c r="E25" s="20">
+        <v>0</v>
+      </c>
+      <c r="F25" s="20">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0</v>
+      </c>
+      <c r="I25" s="20">
         <v>2</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="J25" s="20">
+        <v>0</v>
+      </c>
+      <c r="K25" s="20">
+        <v>0</v>
+      </c>
+      <c r="L25" s="20">
+        <v>0</v>
+      </c>
+      <c r="M25" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="N25" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="O25" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P25" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="16"/>
+    </row>
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>133</v>
       </c>
@@ -1672,22 +2326,47 @@
         <v>161</v>
       </c>
       <c r="D26" s="13">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
         <v>-2</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="N26" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="O26" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H26" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P26" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="16"/>
+    </row>
+    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>136</v>
       </c>
@@ -1698,22 +2377,47 @@
         <v>161</v>
       </c>
       <c r="D27" s="13">
+        <v>0</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
         <v>-1</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0</v>
+      </c>
+      <c r="M27" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="N27" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="O27" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P27" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="16"/>
+    </row>
+    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>139</v>
       </c>
@@ -1726,20 +2430,45 @@
       <c r="D28" s="7">
         <v>0</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0</v>
+      </c>
+      <c r="M28" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="N28" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="O28" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H28" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="P28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>27</v>
       </c>
@@ -1752,20 +2481,45 @@
       <c r="D29" s="17">
         <v>0</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="17">
+        <v>0</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0</v>
+      </c>
+      <c r="G29" s="17">
+        <v>0</v>
+      </c>
+      <c r="H29" s="17">
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <v>0</v>
+      </c>
+      <c r="K29" s="17">
+        <v>0</v>
+      </c>
+      <c r="L29" s="17">
+        <v>0</v>
+      </c>
+      <c r="M29" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="N29" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="O29" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="H29" s="19" t="b">
+      <c r="P29" s="19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q29" s="19"/>
+    </row>
+    <row r="30" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>30</v>
       </c>
@@ -1778,20 +2532,45 @@
       <c r="D30" s="13">
         <v>0</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="13">
+        <v>0</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0</v>
+      </c>
+      <c r="H30" s="13">
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <v>0</v>
+      </c>
+      <c r="J30" s="13">
+        <v>0</v>
+      </c>
+      <c r="K30" s="13">
+        <v>0</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="N30" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="O30" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H30" s="16" t="b">
+      <c r="P30" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q30" s="16"/>
+    </row>
+    <row r="31" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>32</v>
       </c>
@@ -1804,20 +2583,45 @@
       <c r="D31" s="13">
         <v>0</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="13">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13">
+        <v>0</v>
+      </c>
+      <c r="G31" s="13">
+        <v>0</v>
+      </c>
+      <c r="H31" s="13">
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <v>0</v>
+      </c>
+      <c r="J31" s="13">
+        <v>0</v>
+      </c>
+      <c r="K31" s="13">
+        <v>0</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0</v>
+      </c>
+      <c r="M31" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="N31" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="O31" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H31" s="16" t="b">
+      <c r="P31" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q31" s="16"/>
+    </row>
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>34</v>
       </c>
@@ -1828,20 +2632,45 @@
       <c r="D32" s="7">
         <v>0</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0</v>
+      </c>
+      <c r="M32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="N32" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="O32" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H32" s="7" t="b">
+      <c r="P32" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q32" s="7"/>
+    </row>
+    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>36</v>
       </c>
@@ -1852,20 +2681,45 @@
       <c r="D33" s="17">
         <v>0</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="17">
+        <v>0</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0</v>
+      </c>
+      <c r="G33" s="17">
+        <v>0</v>
+      </c>
+      <c r="H33" s="17">
+        <v>0</v>
+      </c>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+      <c r="J33" s="17">
+        <v>0</v>
+      </c>
+      <c r="K33" s="17">
+        <v>0</v>
+      </c>
+      <c r="L33" s="17">
+        <v>0</v>
+      </c>
+      <c r="M33" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="N33" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="O33" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="H33" s="19" t="b">
+      <c r="P33" s="19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q33" s="19"/>
+    </row>
+    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>38</v>
       </c>
@@ -1878,20 +2732,45 @@
       <c r="D34" s="13">
         <v>0</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="13">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0</v>
+      </c>
+      <c r="H34" s="13">
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <v>0</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0</v>
+      </c>
+      <c r="K34" s="13">
+        <v>0</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0</v>
+      </c>
+      <c r="M34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="N34" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="O34" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H34" s="16" t="b">
+      <c r="P34" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
@@ -1904,20 +2783,45 @@
       <c r="D35" s="13">
         <v>0</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="13">
+        <v>0</v>
+      </c>
+      <c r="F35" s="13">
+        <v>0</v>
+      </c>
+      <c r="G35" s="13">
+        <v>0</v>
+      </c>
+      <c r="H35" s="13">
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <v>0</v>
+      </c>
+      <c r="J35" s="13">
+        <v>0</v>
+      </c>
+      <c r="K35" s="13">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0</v>
+      </c>
+      <c r="M35" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="N35" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="O35" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H35" s="16" t="b">
+      <c r="P35" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q35" s="16"/>
+    </row>
+    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>43</v>
       </c>
@@ -1930,20 +2834,45 @@
       <c r="D36" s="13">
         <v>0</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="13">
+        <v>0</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0</v>
+      </c>
+      <c r="J36" s="13">
+        <v>0</v>
+      </c>
+      <c r="K36" s="13">
+        <v>0</v>
+      </c>
+      <c r="L36" s="13">
+        <v>0</v>
+      </c>
+      <c r="M36" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="N36" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="O36" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H36" s="16" t="b">
+      <c r="P36" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q36" s="16"/>
+    </row>
+    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>45</v>
       </c>
@@ -1956,20 +2885,45 @@
       <c r="D37" s="13">
         <v>0</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="13">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <v>0</v>
+      </c>
+      <c r="G37" s="13">
+        <v>0</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0</v>
+      </c>
+      <c r="J37" s="13">
+        <v>0</v>
+      </c>
+      <c r="K37" s="13">
+        <v>0</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0</v>
+      </c>
+      <c r="M37" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="N37" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="O37" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H37" s="16" t="b">
+      <c r="P37" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q37" s="16"/>
+    </row>
+    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
@@ -1982,20 +2936,45 @@
       <c r="D38" s="13">
         <v>0</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="13">
+        <v>0</v>
+      </c>
+      <c r="F38" s="13">
+        <v>0</v>
+      </c>
+      <c r="G38" s="13">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13">
+        <v>0</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0</v>
+      </c>
+      <c r="J38" s="13">
+        <v>0</v>
+      </c>
+      <c r="K38" s="13">
+        <v>0</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0</v>
+      </c>
+      <c r="M38" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="N38" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="O38" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H38" s="16" t="b">
+      <c r="P38" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q38" s="16"/>
+    </row>
+    <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>50</v>
       </c>
@@ -2008,20 +2987,45 @@
       <c r="D39" s="13">
         <v>0</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="13">
+        <v>0</v>
+      </c>
+      <c r="F39" s="13">
+        <v>0</v>
+      </c>
+      <c r="G39" s="13">
+        <v>0</v>
+      </c>
+      <c r="H39" s="13">
+        <v>0</v>
+      </c>
+      <c r="I39" s="13">
+        <v>0</v>
+      </c>
+      <c r="J39" s="13">
+        <v>0</v>
+      </c>
+      <c r="K39" s="13">
+        <v>0</v>
+      </c>
+      <c r="L39" s="13">
+        <v>0</v>
+      </c>
+      <c r="M39" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="N39" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="O39" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H39" s="16" t="b">
+      <c r="P39" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q39" s="16"/>
+    </row>
+    <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>53</v>
       </c>
@@ -2034,20 +3038,45 @@
       <c r="D40" s="13">
         <v>0</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="13">
+        <v>0</v>
+      </c>
+      <c r="F40" s="13">
+        <v>0</v>
+      </c>
+      <c r="G40" s="13">
+        <v>0</v>
+      </c>
+      <c r="H40" s="13">
+        <v>0</v>
+      </c>
+      <c r="I40" s="13">
+        <v>0</v>
+      </c>
+      <c r="J40" s="13">
+        <v>0</v>
+      </c>
+      <c r="K40" s="13">
+        <v>0</v>
+      </c>
+      <c r="L40" s="13">
+        <v>0</v>
+      </c>
+      <c r="M40" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="N40" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G40" s="16" t="s">
+      <c r="O40" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H40" s="16" t="b">
+      <c r="P40" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q40" s="16"/>
+    </row>
+    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>55</v>
       </c>
@@ -2060,20 +3089,45 @@
       <c r="D41" s="13">
         <v>0</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="13">
+        <v>0</v>
+      </c>
+      <c r="F41" s="13">
+        <v>0</v>
+      </c>
+      <c r="G41" s="13">
+        <v>0</v>
+      </c>
+      <c r="H41" s="13">
+        <v>0</v>
+      </c>
+      <c r="I41" s="13">
+        <v>0</v>
+      </c>
+      <c r="J41" s="13">
+        <v>0</v>
+      </c>
+      <c r="K41" s="13">
+        <v>0</v>
+      </c>
+      <c r="L41" s="13">
+        <v>0</v>
+      </c>
+      <c r="M41" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="N41" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="O41" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H41" s="16" t="b">
+      <c r="P41" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q41" s="16"/>
+    </row>
+    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>57</v>
       </c>
@@ -2086,20 +3140,45 @@
       <c r="D42" s="13">
         <v>0</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="13">
+        <v>0</v>
+      </c>
+      <c r="F42" s="13">
+        <v>0</v>
+      </c>
+      <c r="G42" s="13">
+        <v>0</v>
+      </c>
+      <c r="H42" s="13">
+        <v>0</v>
+      </c>
+      <c r="I42" s="13">
+        <v>0</v>
+      </c>
+      <c r="J42" s="13">
+        <v>0</v>
+      </c>
+      <c r="K42" s="13">
+        <v>0</v>
+      </c>
+      <c r="L42" s="13">
+        <v>0</v>
+      </c>
+      <c r="M42" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="N42" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G42" s="16" t="s">
+      <c r="O42" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H42" s="16" t="b">
+      <c r="P42" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q42" s="16"/>
+    </row>
+    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>59</v>
       </c>
@@ -2112,20 +3191,45 @@
       <c r="D43" s="13">
         <v>0</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="13">
+        <v>0</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0</v>
+      </c>
+      <c r="G43" s="13">
+        <v>0</v>
+      </c>
+      <c r="H43" s="13">
+        <v>0</v>
+      </c>
+      <c r="I43" s="13">
+        <v>0</v>
+      </c>
+      <c r="J43" s="13">
+        <v>0</v>
+      </c>
+      <c r="K43" s="13">
+        <v>0</v>
+      </c>
+      <c r="L43" s="13">
+        <v>0</v>
+      </c>
+      <c r="M43" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="N43" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="O43" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H43" s="16" t="b">
+      <c r="P43" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q43" s="16"/>
+    </row>
+    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>61</v>
       </c>
@@ -2138,20 +3242,45 @@
       <c r="D44" s="13">
         <v>0</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="13">
+        <v>0</v>
+      </c>
+      <c r="F44" s="13">
+        <v>0</v>
+      </c>
+      <c r="G44" s="13">
+        <v>0</v>
+      </c>
+      <c r="H44" s="13">
+        <v>0</v>
+      </c>
+      <c r="I44" s="13">
+        <v>0</v>
+      </c>
+      <c r="J44" s="13">
+        <v>0</v>
+      </c>
+      <c r="K44" s="13">
+        <v>0</v>
+      </c>
+      <c r="L44" s="13">
+        <v>0</v>
+      </c>
+      <c r="M44" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="N44" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="O44" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H44" s="16" t="b">
+      <c r="P44" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q44" s="16"/>
+    </row>
+    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>63</v>
       </c>
@@ -2164,20 +3293,45 @@
       <c r="D45" s="13">
         <v>0</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="13">
+        <v>0</v>
+      </c>
+      <c r="F45" s="13">
+        <v>0</v>
+      </c>
+      <c r="G45" s="13">
+        <v>0</v>
+      </c>
+      <c r="H45" s="13">
+        <v>0</v>
+      </c>
+      <c r="I45" s="13">
+        <v>0</v>
+      </c>
+      <c r="J45" s="13">
+        <v>0</v>
+      </c>
+      <c r="K45" s="13">
+        <v>0</v>
+      </c>
+      <c r="L45" s="13">
+        <v>0</v>
+      </c>
+      <c r="M45" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="N45" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="O45" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H45" s="16" t="b">
+      <c r="P45" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q45" s="16"/>
+    </row>
+    <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>65</v>
       </c>
@@ -2190,20 +3344,45 @@
       <c r="D46" s="13">
         <v>0</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="13">
+        <v>0</v>
+      </c>
+      <c r="F46" s="13">
+        <v>0</v>
+      </c>
+      <c r="G46" s="13">
+        <v>0</v>
+      </c>
+      <c r="H46" s="13">
+        <v>0</v>
+      </c>
+      <c r="I46" s="13">
+        <v>0</v>
+      </c>
+      <c r="J46" s="13">
+        <v>0</v>
+      </c>
+      <c r="K46" s="13">
+        <v>0</v>
+      </c>
+      <c r="L46" s="13">
+        <v>0</v>
+      </c>
+      <c r="M46" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="N46" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G46" s="16" t="s">
+      <c r="O46" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H46" s="16" t="b">
+      <c r="P46" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q46" s="16"/>
+    </row>
+    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>67</v>
       </c>
@@ -2216,20 +3395,45 @@
       <c r="D47" s="13">
         <v>0</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="13">
+        <v>0</v>
+      </c>
+      <c r="F47" s="13">
+        <v>0</v>
+      </c>
+      <c r="G47" s="13">
+        <v>0</v>
+      </c>
+      <c r="H47" s="13">
+        <v>0</v>
+      </c>
+      <c r="I47" s="13">
+        <v>0</v>
+      </c>
+      <c r="J47" s="13">
+        <v>0</v>
+      </c>
+      <c r="K47" s="13">
+        <v>0</v>
+      </c>
+      <c r="L47" s="13">
+        <v>0</v>
+      </c>
+      <c r="M47" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="N47" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="O47" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="H47" s="16" t="b">
+      <c r="P47" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q47" s="16"/>
+    </row>
+    <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>69</v>
       </c>
@@ -2240,20 +3444,45 @@
       <c r="D48" s="13">
         <v>0</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="13">
+        <v>0</v>
+      </c>
+      <c r="F48" s="13">
+        <v>0</v>
+      </c>
+      <c r="G48" s="13">
+        <v>0</v>
+      </c>
+      <c r="H48" s="13">
+        <v>0</v>
+      </c>
+      <c r="I48" s="13">
+        <v>0</v>
+      </c>
+      <c r="J48" s="13">
+        <v>0</v>
+      </c>
+      <c r="K48" s="13">
+        <v>0</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0</v>
+      </c>
+      <c r="M48" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="N48" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="O48" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H48" s="16" t="b">
+      <c r="P48" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q48" s="16"/>
+    </row>
+    <row r="49" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>71</v>
       </c>
@@ -2264,20 +3493,45 @@
       <c r="D49" s="13">
         <v>0</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="13">
+        <v>0</v>
+      </c>
+      <c r="F49" s="13">
+        <v>0</v>
+      </c>
+      <c r="G49" s="13">
+        <v>0</v>
+      </c>
+      <c r="H49" s="13">
+        <v>0</v>
+      </c>
+      <c r="I49" s="13">
+        <v>0</v>
+      </c>
+      <c r="J49" s="13">
+        <v>0</v>
+      </c>
+      <c r="K49" s="13">
+        <v>0</v>
+      </c>
+      <c r="L49" s="13">
+        <v>0</v>
+      </c>
+      <c r="M49" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="N49" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="O49" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H49" s="16" t="b">
+      <c r="P49" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q49" s="16"/>
+    </row>
+    <row r="50" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>73</v>
       </c>
@@ -2288,20 +3542,45 @@
       <c r="D50" s="7">
         <v>0</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="7">
+        <v>0</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7">
+        <v>0</v>
+      </c>
+      <c r="J50" s="7">
+        <v>0</v>
+      </c>
+      <c r="K50" s="7">
+        <v>0</v>
+      </c>
+      <c r="L50" s="7">
+        <v>0</v>
+      </c>
+      <c r="M50" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="N50" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="O50" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H50" s="9" t="b">
+      <c r="P50" s="9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q50" s="9"/>
+    </row>
+    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>75</v>
       </c>
@@ -2312,20 +3591,45 @@
       <c r="D51" s="17">
         <v>0</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="17">
+        <v>0</v>
+      </c>
+      <c r="F51" s="17">
+        <v>0</v>
+      </c>
+      <c r="G51" s="17">
+        <v>0</v>
+      </c>
+      <c r="H51" s="17">
+        <v>0</v>
+      </c>
+      <c r="I51" s="17">
+        <v>0</v>
+      </c>
+      <c r="J51" s="17">
+        <v>0</v>
+      </c>
+      <c r="K51" s="17">
+        <v>0</v>
+      </c>
+      <c r="L51" s="17">
+        <v>0</v>
+      </c>
+      <c r="M51" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="N51" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G51" s="19" t="s">
+      <c r="O51" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="H51" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P51" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="19"/>
+    </row>
+    <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>77</v>
       </c>
@@ -2338,20 +3642,45 @@
       <c r="D52" s="13">
         <v>0</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="13">
+        <v>0</v>
+      </c>
+      <c r="F52" s="13">
+        <v>0</v>
+      </c>
+      <c r="G52" s="13">
+        <v>0</v>
+      </c>
+      <c r="H52" s="13">
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
+        <v>0</v>
+      </c>
+      <c r="J52" s="13">
+        <v>0</v>
+      </c>
+      <c r="K52" s="13">
+        <v>0</v>
+      </c>
+      <c r="L52" s="13">
+        <v>0</v>
+      </c>
+      <c r="M52" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="N52" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G52" s="16" t="s">
+      <c r="O52" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H52" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P52" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="16"/>
+    </row>
+    <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>80</v>
       </c>
@@ -2364,20 +3693,45 @@
       <c r="D53" s="13">
         <v>0</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="13">
+        <v>0</v>
+      </c>
+      <c r="F53" s="13">
+        <v>0</v>
+      </c>
+      <c r="G53" s="13">
+        <v>0</v>
+      </c>
+      <c r="H53" s="13">
+        <v>0</v>
+      </c>
+      <c r="I53" s="13">
+        <v>0</v>
+      </c>
+      <c r="J53" s="13">
+        <v>0</v>
+      </c>
+      <c r="K53" s="13">
+        <v>0</v>
+      </c>
+      <c r="L53" s="13">
+        <v>0</v>
+      </c>
+      <c r="M53" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="16" t="s">
+      <c r="N53" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G53" s="16" t="s">
+      <c r="O53" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H53" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P53" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="16"/>
+    </row>
+    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>83</v>
       </c>
@@ -2390,20 +3744,45 @@
       <c r="D54" s="13">
         <v>0</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="13">
+        <v>0</v>
+      </c>
+      <c r="F54" s="13">
+        <v>0</v>
+      </c>
+      <c r="G54" s="13">
+        <v>0</v>
+      </c>
+      <c r="H54" s="13">
+        <v>0</v>
+      </c>
+      <c r="I54" s="13">
+        <v>0</v>
+      </c>
+      <c r="J54" s="13">
+        <v>0</v>
+      </c>
+      <c r="K54" s="13">
+        <v>0</v>
+      </c>
+      <c r="L54" s="13">
+        <v>0</v>
+      </c>
+      <c r="M54" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="16" t="s">
+      <c r="N54" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G54" s="16" t="s">
+      <c r="O54" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H54" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="16"/>
+    </row>
+    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>86</v>
       </c>
@@ -2416,20 +3795,45 @@
       <c r="D55" s="13">
         <v>0</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E55" s="13">
+        <v>0</v>
+      </c>
+      <c r="F55" s="13">
+        <v>0</v>
+      </c>
+      <c r="G55" s="13">
+        <v>0</v>
+      </c>
+      <c r="H55" s="13">
+        <v>0</v>
+      </c>
+      <c r="I55" s="13">
+        <v>0</v>
+      </c>
+      <c r="J55" s="13">
+        <v>0</v>
+      </c>
+      <c r="K55" s="13">
+        <v>0</v>
+      </c>
+      <c r="L55" s="13">
+        <v>0</v>
+      </c>
+      <c r="M55" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="N55" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G55" s="16" t="s">
+      <c r="O55" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H55" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="P55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="16"/>
+    </row>
+    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>89</v>
       </c>
@@ -2442,20 +3846,45 @@
       <c r="D56" s="13">
         <v>0</v>
       </c>
-      <c r="E56" s="15" t="s">
+      <c r="E56" s="13">
+        <v>0</v>
+      </c>
+      <c r="F56" s="13">
+        <v>0</v>
+      </c>
+      <c r="G56" s="13">
+        <v>0</v>
+      </c>
+      <c r="H56" s="13">
+        <v>0</v>
+      </c>
+      <c r="I56" s="13">
+        <v>0</v>
+      </c>
+      <c r="J56" s="13">
+        <v>0</v>
+      </c>
+      <c r="K56" s="13">
+        <v>0</v>
+      </c>
+      <c r="L56" s="13">
+        <v>0</v>
+      </c>
+      <c r="M56" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F56" s="16" t="s">
+      <c r="N56" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G56" s="16" t="s">
+      <c r="O56" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H56" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="P56" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="16"/>
+    </row>
+    <row r="57" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>92</v>
       </c>
@@ -2468,20 +3897,45 @@
       <c r="D57" s="13">
         <v>0</v>
       </c>
-      <c r="E57" s="15" t="s">
+      <c r="E57" s="13">
+        <v>0</v>
+      </c>
+      <c r="F57" s="13">
+        <v>0</v>
+      </c>
+      <c r="G57" s="13">
+        <v>0</v>
+      </c>
+      <c r="H57" s="13">
+        <v>0</v>
+      </c>
+      <c r="I57" s="13">
+        <v>0</v>
+      </c>
+      <c r="J57" s="13">
+        <v>0</v>
+      </c>
+      <c r="K57" s="13">
+        <v>0</v>
+      </c>
+      <c r="L57" s="13">
+        <v>0</v>
+      </c>
+      <c r="M57" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="N57" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G57" s="16" t="s">
+      <c r="O57" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H57" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="P57" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="16"/>
+    </row>
+    <row r="58" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>95</v>
       </c>
@@ -2494,18 +3948,43 @@
       <c r="D58" s="7">
         <v>0</v>
       </c>
-      <c r="E58" s="22" t="s">
+      <c r="E58" s="7">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0</v>
+      </c>
+      <c r="J58" s="7">
+        <v>0</v>
+      </c>
+      <c r="K58" s="7">
+        <v>0</v>
+      </c>
+      <c r="L58" s="7">
+        <v>0</v>
+      </c>
+      <c r="M58" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="N58" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="O58" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H58" s="7" t="b">
-        <v>0</v>
-      </c>
+      <c r="P58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>